<commit_message>
revisions required for new jlcpcb submission
</commit_message>
<xml_diff>
--- a/MANUFACTURE/F405_pill-top-pos.xlsx
+++ b/MANUFACTURE/F405_pill-top-pos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/Documents/kicad /F405_pill/GERBERS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/kicad/F405_pill/MANUFACTURE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2B57F6-8EA5-2E4B-89AC-B467CF6233AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFC2EFA-DBA6-D84C-9270-AD9BD5C9E562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="15400" yWindow="6480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F405_pill-top-pos" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Package</t>
   </si>
   <si>
-    <t>Side</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -217,7 +214,7 @@
     <t>STM32F405RGTx</t>
   </si>
   <si>
-    <t>LQFP-64_10x10mm_P0.5mm</t>
+    <t>my_STM32F405RGTx_2</t>
   </si>
   <si>
     <t>U2</t>
@@ -257,12 +254,15 @@
   </si>
   <si>
     <t>Rotation</t>
+  </si>
+  <si>
+    <t>Layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -740,9 +740,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1097,47 +1096,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>120.887</v>
@@ -1149,18 +1148,18 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>120.62</v>
@@ -1172,18 +1171,18 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>123.414</v>
@@ -1195,18 +1194,18 @@
         <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
       <c r="D5">
         <v>118.514</v>
@@ -1218,18 +1217,18 @@
         <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>121</v>
@@ -1241,18 +1240,18 @@
         <v>-90</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>123.541</v>
@@ -1264,18 +1263,18 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
       <c r="D8">
         <v>107.03100000000001</v>
@@ -1287,18 +1286,18 @@
         <v>180</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>119.858</v>
@@ -1310,18 +1309,18 @@
         <v>-90</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>105.00700000000001</v>
@@ -1333,18 +1332,18 @@
         <v>-90</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
       </c>
       <c r="D11">
         <v>106.617</v>
@@ -1356,18 +1355,18 @@
         <v>-90</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>104.901</v>
@@ -1379,18 +1378,18 @@
         <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
       </c>
       <c r="D13">
         <v>118.58799999999999</v>
@@ -1402,18 +1401,18 @@
         <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>144.6</v>
@@ -1425,18 +1424,18 @@
         <v>-90</v>
       </c>
       <c r="G14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>141.47999999999999</v>
@@ -1448,18 +1447,18 @@
         <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>141.47999999999999</v>
@@ -1471,18 +1470,18 @@
         <v>-90</v>
       </c>
       <c r="G16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
       </c>
       <c r="D17">
         <v>142.30000000000001</v>
@@ -1494,18 +1493,18 @@
         <v>-90</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
       </c>
       <c r="D18">
         <v>124.68</v>
@@ -1517,18 +1516,18 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
       </c>
       <c r="D19">
         <v>124.68</v>
@@ -1540,18 +1539,18 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
         <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
       </c>
       <c r="D20">
         <v>119.86</v>
@@ -1563,18 +1562,18 @@
         <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>143.30000000000001</v>
@@ -1586,18 +1585,18 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
       </c>
       <c r="D22">
         <v>100.23699999999999</v>
@@ -1609,18 +1608,18 @@
         <v>180</v>
       </c>
       <c r="G22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>100.24</v>
@@ -1632,18 +1631,18 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
       </c>
       <c r="D24">
         <v>131.68199999999999</v>
@@ -1655,18 +1654,18 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
       </c>
       <c r="D25">
         <v>95.682000000000002</v>
@@ -1678,18 +1677,18 @@
         <v>-90</v>
       </c>
       <c r="G25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
       </c>
       <c r="D26">
         <v>121</v>
@@ -1701,18 +1700,18 @@
         <v>-90</v>
       </c>
       <c r="G26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>51</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
       </c>
       <c r="D27">
         <v>125.989</v>
@@ -1724,18 +1723,18 @@
         <v>-90</v>
       </c>
       <c r="G27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
       </c>
       <c r="D28">
         <v>127.56399999999999</v>
@@ -1747,18 +1746,18 @@
         <v>180</v>
       </c>
       <c r="G28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>143.21799999999999</v>
@@ -1770,18 +1769,18 @@
         <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30">
         <v>143.21799999999999</v>
@@ -1793,18 +1792,18 @@
         <v>90</v>
       </c>
       <c r="G30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
         <v>57</v>
       </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31">
         <v>103.33199999999999</v>
@@ -1816,18 +1815,18 @@
         <v>180</v>
       </c>
       <c r="G31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
         <v>51</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
       </c>
       <c r="D32">
         <v>131.78200000000001</v>
@@ -1839,18 +1838,18 @@
         <v>-90</v>
       </c>
       <c r="G32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
-        <v>61</v>
-      </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33">
         <v>97.096000000000004</v>
@@ -1862,18 +1861,18 @@
         <v>90</v>
       </c>
       <c r="G33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34">
         <v>97.096000000000004</v>
@@ -1885,18 +1884,18 @@
         <v>-90</v>
       </c>
       <c r="G34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>64</v>
-      </c>
-      <c r="C35" t="s">
-        <v>65</v>
       </c>
       <c r="D35">
         <v>112.492</v>
@@ -1905,21 +1904,21 @@
         <v>-84.679000000000002</v>
       </c>
       <c r="F35">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="G35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
         <v>66</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>67</v>
-      </c>
-      <c r="C36" t="s">
-        <v>68</v>
       </c>
       <c r="D36">
         <v>137.04202799999999</v>
@@ -1931,18 +1930,18 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
         <v>69</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
       </c>
       <c r="D37">
         <v>136.18199999999999</v>
@@ -1954,18 +1953,18 @@
         <v>180</v>
       </c>
       <c r="G37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>73</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
       </c>
       <c r="D38">
         <v>123.33</v>
@@ -1977,7 +1976,7 @@
         <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>